<commit_message>
Update to shorter help messages
</commit_message>
<xml_diff>
--- a/src/index spreadsheet/HELP MNUs.xlsx
+++ b/src/index spreadsheet/HELP MNUs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacomostert/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacomostert/wp43s/src/index spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99296E8-A546-1F49-A8C7-35CB808E4E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC10AFF3-CEC0-8F4A-AA10-20DCD18ADC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="2840" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{5C31C776-C7DF-CC47-8195-6B9461F090FC}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="571">
   <si>
     <t>ITEM</t>
   </si>
@@ -1742,9 +1742,6 @@
   </si>
   <si>
     <t>XXEQ menu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      {0,MNU_HOME,   "This is the HOME page draft help page.\n"},</t>
   </si>
 </sst>
 </file>
@@ -4812,8 +4809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49219A7-1CA1-9843-9665-39F5940DB55D}">
   <dimension ref="A1:A161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4822,961 +4819,959 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="7" t="s">
-        <v>571</v>
-      </c>
+      <c r="A1" s="7"/>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="str">
-        <f>IF(MID(Sheet1!A2,1,3)="MNU","{0,"&amp;Sheet1!A2&amp;",   """&amp;Sheet1!E2&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A2,1,3)="MNU",MID(Sheet1!A2,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A2&amp;",   """&amp;Sheet1!D2&amp;"\n""},","")</f>
         <v>{0,MNU_Sf,   "Integral f\n"},</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="str">
-        <f>IF(MID(Sheet1!A3,1,3)="MNU","{0,"&amp;Sheet1!A3&amp;",   """&amp;Sheet1!E3&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A3,1,3)="MNU",MID(Sheet1!A3,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A3&amp;",   """&amp;Sheet1!D3&amp;"\n""},","")</f>
         <v>{0,MNU_Sfdx,   "Integral f dx\n"},</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="str">
-        <f>IF(MID(Sheet1!A4,1,3)="MNU","{0,"&amp;Sheet1!A4&amp;",   """&amp;Sheet1!E4&amp;"\n""},","")</f>
-        <v>{0,MNU_ADV,   "Advanced functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A4,1,3)="MNU",MID(Sheet1!A4,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A4&amp;",   """&amp;Sheet1!D4&amp;"\n""},","")</f>
+        <v>{0,MNU_ADV,   "Advanced\n"},</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="str">
-        <f>IF(MID(Sheet1!A5,1,3)="MNU","{0,"&amp;Sheet1!A5&amp;",   """&amp;Sheet1!E5&amp;"\n""},","")</f>
-        <v>{0,MNU_CONVANG,   "Convert between units of angle\n"},</v>
+        <f>IF(AND(MID(Sheet1!A5,1,3)="MNU",MID(Sheet1!A5,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A5&amp;",   """&amp;Sheet1!D5&amp;"\n""},","")</f>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="str">
-        <f>IF(MID(Sheet1!A6,1,3)="MNU","{0,"&amp;Sheet1!A6&amp;",   """&amp;Sheet1!E6&amp;"\n""},","")</f>
-        <v>{0,MNU_ANGLES,   "Auto-generated catalog of variables of the specified type: angle\n"},</v>
+        <f>IF(AND(MID(Sheet1!A6,1,3)="MNU",MID(Sheet1!A6,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A6&amp;",   """&amp;Sheet1!D6&amp;"\n""},","")</f>
+        <v>{0,MNU_ANGLES,   "Angle variables\n"},</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="str">
-        <f>IF(MID(Sheet1!A7,1,3)="MNU","{0,"&amp;Sheet1!A7&amp;",   """&amp;Sheet1!E7&amp;"\n""},","")</f>
-        <v>{0,MNU_CONVA,   "Convert between units of area\n"},</v>
+        <f>IF(AND(MID(Sheet1!A7,1,3)="MNU",MID(Sheet1!A7,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A7&amp;",   """&amp;Sheet1!D7&amp;"\n""},","")</f>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="str">
-        <f>IF(MID(Sheet1!A8,1,3)="MNU","{0,"&amp;Sheet1!A8&amp;",   """&amp;Sheet1!E8&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A8,1,3)="MNU",MID(Sheet1!A8,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A8&amp;",   """&amp;Sheet1!D8&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="str">
-        <f>IF(MID(Sheet1!A9,1,3)="MNU","{0,"&amp;Sheet1!A9&amp;",   """&amp;Sheet1!E9&amp;"\n""},","")</f>
-        <v>{0,MNU_PLOT_LR,   "Assess curve fitting\n"},</v>
+        <f>IF(AND(MID(Sheet1!A9,1,3)="MNU",MID(Sheet1!A9,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A9&amp;",   """&amp;Sheet1!D9&amp;"\n""},","")</f>
+        <v>{0,MNU_PLOT_LR,   "Assess\n"},</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="str">
-        <f>IF(MID(Sheet1!A10,1,3)="MNU","{0,"&amp;Sheet1!A10&amp;",   """&amp;Sheet1!E10&amp;"\n""},","")</f>
-        <v>{0,MNU_BASE,   "Number base operations\n"},</v>
+        <f>IF(AND(MID(Sheet1!A10,1,3)="MNU",MID(Sheet1!A10,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A10&amp;",   """&amp;Sheet1!D10&amp;"\n""},","")</f>
+        <v>{0,MNU_BASE,   "Number base\n"},</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="str">
-        <f>IF(MID(Sheet1!A11,1,3)="MNU","{0,"&amp;Sheet1!A11&amp;",   """&amp;Sheet1!E11&amp;"\n""},","")</f>
-        <v>{0,MNU_BINOM,   "Binomial probability distribution\n"},</v>
+        <f>IF(AND(MID(Sheet1!A11,1,3)="MNU",MID(Sheet1!A11,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A11&amp;",   """&amp;Sheet1!D11&amp;"\n""},","")</f>
+        <v>{0,MNU_BINOM,   "Binomial distribution\n"},</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="str">
-        <f>IF(MID(Sheet1!A12,1,3)="MNU","{0,"&amp;Sheet1!A12&amp;",   """&amp;Sheet1!E12&amp;"\n""},","")</f>
-        <v>{0,MNU_BITS,   "Bitwise operations\n"},</v>
+        <f>IF(AND(MID(Sheet1!A12,1,3)="MNU",MID(Sheet1!A12,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A12&amp;",   """&amp;Sheet1!D12&amp;"\n""},","")</f>
+        <v>{0,MNU_BITS,   "Bits\n"},</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="str">
-        <f>IF(MID(Sheet1!A13,1,3)="MNU","{0,"&amp;Sheet1!A13&amp;",   """&amp;Sheet1!E13&amp;"\n""},","")</f>
-        <v>{0,MNU_BLUE_C47,   "Access all C47 gShifted functions and a few fShifted, supporting layout DM42\n"},</v>
+        <f>IF(AND(MID(Sheet1!A13,1,3)="MNU",MID(Sheet1!A13,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A13&amp;",   """&amp;Sheet1!D13&amp;"\n""},","")</f>
+        <v>{0,MNU_BLUE_C47,   "Access blue functions\n"},</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="str">
-        <f>IF(MID(Sheet1!A14,1,3)="MNU","{0,"&amp;Sheet1!A14&amp;",   """&amp;Sheet1!E14&amp;"\n""},","")</f>
-        <v>{0,MNU_CATALOG,   "Catalog of all items (functions, characters, programs, variables, menus)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A14,1,3)="MNU",MID(Sheet1!A14,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A14&amp;",   """&amp;Sheet1!D14&amp;"\n""},","")</f>
+        <v>{0,MNU_CATALOG,   "Catalog\n"},</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="str">
-        <f>IF(MID(Sheet1!A15,1,3)="MNU","{0,"&amp;Sheet1!A15&amp;",   """&amp;Sheet1!E15&amp;"\n""},","")</f>
-        <v>{0,MNU_CAUCH,   "Cauchy-Lorentz probability distribution\n"},</v>
+        <f>IF(AND(MID(Sheet1!A15,1,3)="MNU",MID(Sheet1!A15,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A15&amp;",   """&amp;Sheet1!D15&amp;"\n""},","")</f>
+        <v>{0,MNU_CAUCH,   "Cauchy-Lorentz distribution\n"},</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="str">
-        <f>IF(MID(Sheet1!A16,1,3)="MNU","{0,"&amp;Sheet1!A16&amp;",   """&amp;Sheet1!E16&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A16,1,3)="MNU",MID(Sheet1!A16,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A16&amp;",   """&amp;Sheet1!D16&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="str">
-        <f>IF(MID(Sheet1!A17,1,3)="MNU","{0,"&amp;Sheet1!A17&amp;",   """&amp;Sheet1!E17&amp;"\n""},","")</f>
-        <v>{0,MNU_CHARS,   "Access to all character submenus (international, greek, math, MyAlpha, alphaDot)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A17,1,3)="MNU",MID(Sheet1!A17,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A17&amp;",   """&amp;Sheet1!D17&amp;"\n""},","")</f>
+        <v>{0,MNU_CHARS,   "Characters\n"},</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="str">
-        <f>IF(MID(Sheet1!A18,1,3)="MNU","{0,"&amp;Sheet1!A18&amp;",   """&amp;Sheet1!E18&amp;"\n""},","")</f>
-        <v>{0,MNU_CLK,   "Clock functions, including setting date and time and julian day numbers (astronomy)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A18,1,3)="MNU",MID(Sheet1!A18,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A18&amp;",   """&amp;Sheet1!D18&amp;"\n""},","")</f>
+        <v>{0,MNU_CLK,   "Clock\n"},</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="str">
-        <f>IF(MID(Sheet1!A19,1,3)="MNU","{0,"&amp;Sheet1!A19&amp;",   """&amp;Sheet1!E19&amp;"\n""},","")</f>
-        <v>{0,MNU_CLR,   "Clear flags, programs, registers, stacks, variables and reset calculator\n"},</v>
+        <f>IF(AND(MID(Sheet1!A19,1,3)="MNU",MID(Sheet1!A19,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A19&amp;",   """&amp;Sheet1!D19&amp;"\n""},","")</f>
+        <v>{0,MNU_CLR,   "Clear\n"},</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="str">
-        <f>IF(MID(Sheet1!A20,1,3)="MNU","{0,"&amp;Sheet1!A20&amp;",   """&amp;Sheet1!E20&amp;"\n""},","")</f>
-        <v>{0,MNU_CONST,   "Important scientific and technical constant values\n"},</v>
+        <f>IF(AND(MID(Sheet1!A20,1,3)="MNU",MID(Sheet1!A20,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A20&amp;",   """&amp;Sheet1!D20&amp;"\n""},","")</f>
+        <v>{0,MNU_CONST,   "Constants\n"},</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="str">
-        <f>IF(MID(Sheet1!A21,1,3)="MNU","{0,"&amp;Sheet1!A21&amp;",   """&amp;Sheet1!E21&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A21,1,3)="MNU",MID(Sheet1!A21,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A21&amp;",   """&amp;Sheet1!D21&amp;"\n""},","")</f>
         <v>{0,MNU_UNITCONV,   "Convert units\n"},</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="str">
-        <f>IF(MID(Sheet1!A22,1,3)="MNU","{0,"&amp;Sheet1!A22&amp;",   """&amp;Sheet1!E22&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A22,1,3)="MNU",MID(Sheet1!A22,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A22&amp;",   """&amp;Sheet1!D22&amp;"\n""},","")</f>
         <v>{0,MNU_ANGLECONV_C43,   "Convert angles\n"},</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="str">
-        <f>IF(MID(Sheet1!A23,1,3)="MNU","{0,"&amp;Sheet1!A23&amp;",   """&amp;Sheet1!E23&amp;"\n""},","")</f>
-        <v>{0,MNU_CPX,   "Complex functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A23,1,3)="MNU",MID(Sheet1!A23,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A23&amp;",   """&amp;Sheet1!D23&amp;"\n""},","")</f>
+        <v>{0,MNU_CPX,   "Complex\n"},</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="str">
-        <f>IF(MID(Sheet1!A24,1,3)="MNU","{0,"&amp;Sheet1!A24&amp;",   """&amp;Sheet1!E24&amp;"\n""},","")</f>
-        <v>{0,MNU_CPXS,   "Auto-generated catalog of variables of the specified type: complex\n"},</v>
+        <f>IF(AND(MID(Sheet1!A24,1,3)="MNU",MID(Sheet1!A24,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A24&amp;",   """&amp;Sheet1!D24&amp;"\n""},","")</f>
+        <v>{0,MNU_CPXS,   "Complex variables\n"},</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="str">
-        <f>IF(MID(Sheet1!A25,1,3)="MNU","{0,"&amp;Sheet1!A25&amp;",   """&amp;Sheet1!E25&amp;"\n""},","")</f>
-        <v>{0,MNU_DATES,   "Auto-generated catalog of variables of the specified type: date\n"},</v>
+        <f>IF(AND(MID(Sheet1!A25,1,3)="MNU",MID(Sheet1!A25,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A25&amp;",   """&amp;Sheet1!D25&amp;"\n""},","")</f>
+        <v>{0,MNU_DATES,   "Date variables\n"},</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="str">
-        <f>IF(MID(Sheet1!A26,1,3)="MNU","{0,"&amp;Sheet1!A26&amp;",   """&amp;Sheet1!E26&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A26,1,3)="MNU",MID(Sheet1!A26,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A26&amp;",   """&amp;Sheet1!D26&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="str">
-        <f>IF(MID(Sheet1!A27,1,3)="MNU","{0,"&amp;Sheet1!A27&amp;",   """&amp;Sheet1!E27&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A27,1,3)="MNU",MID(Sheet1!A27,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A27&amp;",   """&amp;Sheet1!D27&amp;"\n""},","")</f>
         <v>{0,MNU_DISP,   "Display settings\n"},</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="str">
-        <f>IF(MID(Sheet1!A28,1,3)="MNU","{0,"&amp;Sheet1!A28&amp;",   """&amp;Sheet1!E28&amp;"\n""},","")</f>
-        <v>{0,MNU_CONVX,   "Convert between units of distance\n"},</v>
+        <f>IF(AND(MID(Sheet1!A28,1,3)="MNU",MID(Sheet1!A28,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A28&amp;",   """&amp;Sheet1!D28&amp;"\n""},","")</f>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="str">
-        <f>IF(MID(Sheet1!A29,1,3)="MNU","{0,"&amp;Sheet1!A29&amp;",   """&amp;Sheet1!E29&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A29,1,3)="MNU",MID(Sheet1!A29,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A29&amp;",   """&amp;Sheet1!D29&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="str">
-        <f>IF(MID(Sheet1!A30,1,3)="MNU","{0,"&amp;Sheet1!A30&amp;",   """&amp;Sheet1!E30&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A30,1,3)="MNU",MID(Sheet1!A30,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A30&amp;",   """&amp;Sheet1!D30&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="str">
-        <f>IF(MID(Sheet1!A31,1,3)="MNU","{0,"&amp;Sheet1!A31&amp;",   """&amp;Sheet1!E31&amp;"\n""},","")</f>
-        <v>{0,MNU_M_EDIT,   "Matrix edit functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A31,1,3)="MNU",MID(Sheet1!A31,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A31&amp;",   """&amp;Sheet1!D31&amp;"\n""},","")</f>
+        <v>{0,MNU_M_EDIT,   "Matrix editor\n"},</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="str">
-        <f>IF(MID(Sheet1!A32,1,3)="MNU","{0,"&amp;Sheet1!A32&amp;",   """&amp;Sheet1!E32&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A32,1,3)="MNU",MID(Sheet1!A32,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A32&amp;",   """&amp;Sheet1!D32&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="str">
-        <f>IF(MID(Sheet1!A33,1,3)="MNU","{0,"&amp;Sheet1!A33&amp;",   """&amp;Sheet1!E33&amp;"\n""},","")</f>
-        <v>{0,MNU_EE,   "Electrical engineering functions and custom programs\n"},</v>
+        <f>IF(AND(MID(Sheet1!A33,1,3)="MNU",MID(Sheet1!A33,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A33&amp;",   """&amp;Sheet1!D33&amp;"\n""},","")</f>
+        <v>{0,MNU_EE,   "Electrical engineering\n"},</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="str">
-        <f>IF(MID(Sheet1!A34,1,3)="MNU","{0,"&amp;Sheet1!A34&amp;",   """&amp;Sheet1!E34&amp;"\n""},","")</f>
-        <v>{0,MNU_ELLIPT,   "Elliptical functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A34,1,3)="MNU",MID(Sheet1!A34,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A34&amp;",   """&amp;Sheet1!D34&amp;"\n""},","")</f>
+        <v>{0,MNU_ELLIPT,   "Eliiptical\n"},</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="str">
-        <f>IF(MID(Sheet1!A35,1,3)="MNU","{0,"&amp;Sheet1!A35&amp;",   """&amp;Sheet1!E35&amp;"\n""},","")</f>
-        <v>{0,MNU_CONVE,   "Convert between units of energy\n"},</v>
+        <f>IF(AND(MID(Sheet1!A35,1,3)="MNU",MID(Sheet1!A35,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A35&amp;",   """&amp;Sheet1!D35&amp;"\n""},","")</f>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="str">
-        <f>IF(MID(Sheet1!A36,1,3)="MNU","{0,"&amp;Sheet1!A36&amp;",   """&amp;Sheet1!E36&amp;"\n""},","")</f>
-        <v>{0,MNU_EQN,   "Equation editor\n"},</v>
+        <f>IF(AND(MID(Sheet1!A36,1,3)="MNU",MID(Sheet1!A36,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A36&amp;",   """&amp;Sheet1!D36&amp;"\n""},","")</f>
+        <v>{0,MNU_EQN,   "Equation\n"},</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="str">
-        <f>IF(MID(Sheet1!A37,1,3)="MNU","{0,"&amp;Sheet1!A37&amp;",   """&amp;Sheet1!E37&amp;"\n""},","")</f>
-        <v>{0,MNU_EXP,   "Exponential functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A37,1,3)="MNU",MID(Sheet1!A37,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A37&amp;",   """&amp;Sheet1!D37&amp;"\n""},","")</f>
+        <v>{0,MNU_EXP,   "Exponential\n"},</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="str">
-        <f>IF(MID(Sheet1!A38,1,3)="MNU","{0,"&amp;Sheet1!A38&amp;",   """&amp;Sheet1!E38&amp;"\n""},","")</f>
-        <v>{0,MNU_EXPON,   "Exponential probability distribution\n"},</v>
+        <f>IF(AND(MID(Sheet1!A38,1,3)="MNU",MID(Sheet1!A38,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A38&amp;",   """&amp;Sheet1!D38&amp;"\n""},","")</f>
+        <v>{0,MNU_EXPON,   "Exponential distribution\n"},</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="str">
-        <f>IF(MID(Sheet1!A39,1,3)="MNU","{0,"&amp;Sheet1!A39&amp;",   """&amp;Sheet1!E39&amp;"\n""},","")</f>
-        <v>{0,MNU_F,   "Fisher's F probability distribution\n"},</v>
+        <f>IF(AND(MID(Sheet1!A39,1,3)="MNU",MID(Sheet1!A39,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A39&amp;",   """&amp;Sheet1!D39&amp;"\n""},","")</f>
+        <v>{0,MNU_F,   "Fisher's F distribution\n"},</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="str">
-        <f>IF(MID(Sheet1!A40,1,3)="MNU","{0,"&amp;Sheet1!A40&amp;",   """&amp;Sheet1!E40&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A40,1,3)="MNU",MID(Sheet1!A40,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A40&amp;",   """&amp;Sheet1!D40&amp;"\n""},","")</f>
         <v>{0,MNU_1STDERIV,   "First derivative\n"},</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="str">
-        <f>IF(MID(Sheet1!A41,1,3)="MNU","{0,"&amp;Sheet1!A41&amp;",   """&amp;Sheet1!E41&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A41,1,3)="MNU",MID(Sheet1!A41,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A41&amp;",   """&amp;Sheet1!D41&amp;"\n""},","")</f>
         <v>{0,MNU_2NDDERIV,   "Second derivative\n"},</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="str">
-        <f>IF(MID(Sheet1!A42,1,3)="MNU","{0,"&amp;Sheet1!A42&amp;",   """&amp;Sheet1!E42&amp;"\n""},","")</f>
-        <v>{0,MNU_CONVFP,   "Convert between units of force and pressure\n"},</v>
+        <f>IF(AND(MID(Sheet1!A42,1,3)="MNU",MID(Sheet1!A42,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A42&amp;",   """&amp;Sheet1!D42&amp;"\n""},","")</f>
+        <v/>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="str">
-        <f>IF(MID(Sheet1!A43,1,3)="MNU","{0,"&amp;Sheet1!A43&amp;",   """&amp;Sheet1!E43&amp;"\n""},","")</f>
-        <v>{0,MNU_FCNS,   "Catalog of all calculator functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A43,1,3)="MNU",MID(Sheet1!A43,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A43&amp;",   """&amp;Sheet1!D43&amp;"\n""},","")</f>
+        <v>{0,MNU_FCNS,   "Functions\n"},</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="str">
-        <f>IF(MID(Sheet1!A44,1,3)="MNU","{0,"&amp;Sheet1!A44&amp;",   """&amp;Sheet1!E44&amp;"\n""},","")</f>
-        <v>{0,MNU_CONVHUM,   "Conversions to and from the furlong-firkin-fortnight (FFF) system (and beardseconds)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A44,1,3)="MNU",MID(Sheet1!A44,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A44&amp;",   """&amp;Sheet1!D44&amp;"\n""},","")</f>
+        <v/>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="str">
-        <f>IF(MID(Sheet1!A45,1,3)="MNU","{0,"&amp;Sheet1!A45&amp;",   """&amp;Sheet1!E45&amp;"\n""},","")</f>
-        <v>{0,MNU_FIN,   "Financial calculations including time value of money (TVM)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A45,1,3)="MNU",MID(Sheet1!A45,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A45&amp;",   """&amp;Sheet1!D45&amp;"\n""},","")</f>
+        <v>{0,MNU_FIN,   "Financial\n"},</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="str">
-        <f>IF(MID(Sheet1!A46,1,3)="MNU","{0,"&amp;Sheet1!A46&amp;",   """&amp;Sheet1!E46&amp;"\n""},","")</f>
-        <v>{0,MNU_FLAGS,   "Setting, clearing and testing flags\n"},</v>
+        <f>IF(AND(MID(Sheet1!A46,1,3)="MNU",MID(Sheet1!A46,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A46&amp;",   """&amp;Sheet1!D46&amp;"\n""},","")</f>
+        <v>{0,MNU_FLAGS,   "Flags\n"},</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="str">
-        <f>IF(MID(Sheet1!A47,1,3)="MNU","{0,"&amp;Sheet1!A47&amp;",   """&amp;Sheet1!E47&amp;"\n""},","")</f>
-        <v>{0,MNU_FLASH,   "Auto-generated catalog of programs in FLASH memory\n"},</v>
+        <f>IF(AND(MID(Sheet1!A47,1,3)="MNU",MID(Sheet1!A47,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A47&amp;",   """&amp;Sheet1!D47&amp;"\n""},","")</f>
+        <v>{0,MNU_FLASH,   "FLASH programs\n"},</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="str">
-        <f>IF(MID(Sheet1!A48,1,3)="MNU","{0,"&amp;Sheet1!A48&amp;",   """&amp;Sheet1!E48&amp;"\n""},","")</f>
-        <v>{0,MNU_GAP_R,   "Select fractional part separator\n"},</v>
+        <f>IF(AND(MID(Sheet1!A48,1,3)="MNU",MID(Sheet1!A48,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A48&amp;",   """&amp;Sheet1!D48&amp;"\n""},","")</f>
+        <v>{0,MNU_GAP_R,   "Select FP separator\n"},</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="str">
-        <f>IF(MID(Sheet1!A49,1,3)="MNU","{0,"&amp;Sheet1!A49&amp;",   """&amp;Sheet1!E49&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A49,1,3)="MNU",MID(Sheet1!A49,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A49&amp;",   """&amp;Sheet1!D49&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="str">
-        <f>IF(MID(Sheet1!A50,1,3)="MNU","{0,"&amp;Sheet1!A50&amp;",   """&amp;Sheet1!E50&amp;"\n""},","")</f>
-        <v>{0,MNU_GEOM,   "Geometric probability distribution\n"},</v>
+        <f>IF(AND(MID(Sheet1!A50,1,3)="MNU",MID(Sheet1!A50,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A50&amp;",   """&amp;Sheet1!D50&amp;"\n""},","")</f>
+        <v>{0,MNU_GEOM,   "Geometric distribution\n"},</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="str">
-        <f>IF(MID(Sheet1!A51,1,3)="MNU","{0,"&amp;Sheet1!A51&amp;",   """&amp;Sheet1!E51&amp;"\n""},","")</f>
-        <v>{0,MNU_GRAPH,   "Graphing functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A51,1,3)="MNU",MID(Sheet1!A51,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A51&amp;",   """&amp;Sheet1!D51&amp;"\n""},","")</f>
+        <v>{0,MNU_GRAPH,   "Graphing\n"},</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="str">
-        <f>IF(MID(Sheet1!A52,1,3)="MNU","{0,"&amp;Sheet1!A52&amp;",   """&amp;Sheet1!E52&amp;"\n""},","")</f>
-        <v>{0,MNU_HIST,   "Histogram functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A52,1,3)="MNU",MID(Sheet1!A52,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A52&amp;",   """&amp;Sheet1!D52&amp;"\n""},","")</f>
+        <v>{0,MNU_HIST,   "Histogram\n"},</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="str">
-        <f>IF(MID(Sheet1!A53,1,3)="MNU","{0,"&amp;Sheet1!A53&amp;",   """&amp;Sheet1!E53&amp;"\n""},","")</f>
-        <v>{0,MNU_HOME,   "HOME menu\n"},</v>
+        <f>IF(AND(MID(Sheet1!A53,1,3)="MNU",MID(Sheet1!A53,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A53&amp;",   """&amp;Sheet1!D53&amp;"\n""},","")</f>
+        <v>{0,MNU_HOME,   "HOME\n"},</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="str">
-        <f>IF(MID(Sheet1!A54,1,3)="MNU","{0,"&amp;Sheet1!A54&amp;",   """&amp;Sheet1!E54&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A54,1,3)="MNU",MID(Sheet1!A54,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A54&amp;",   """&amp;Sheet1!D54&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="str">
-        <f>IF(MID(Sheet1!A55,1,3)="MNU","{0,"&amp;Sheet1!A55&amp;",   """&amp;Sheet1!E55&amp;"\n""},","")</f>
-        <v>{0,MNU_HPLOT,   "Histogram plotting\n"},</v>
+        <f>IF(AND(MID(Sheet1!A55,1,3)="MNU",MID(Sheet1!A55,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A55&amp;",   """&amp;Sheet1!D55&amp;"\n""},","")</f>
+        <v>{0,MNU_HPLOT,   "Histogram\n"},</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="str">
-        <f>IF(MID(Sheet1!A56,1,3)="MNU","{0,"&amp;Sheet1!A56&amp;",   """&amp;Sheet1!E56&amp;"\n""},","")</f>
-        <v>{0,MNU_HYPER,   "Hypergeometric probability distribution\n"},</v>
+        <f>IF(AND(MID(Sheet1!A56,1,3)="MNU",MID(Sheet1!A56,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A56&amp;",   """&amp;Sheet1!D56&amp;"\n""},","")</f>
+        <v>{0,MNU_HYPER,   "Hypergeometric distribution\n"},</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="str">
-        <f>IF(MID(Sheet1!A57,1,3)="MNU","{0,"&amp;Sheet1!A57&amp;",   """&amp;Sheet1!E57&amp;"\n""},","")</f>
-        <v>{0,MNU_IO,   "Input/output functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A57,1,3)="MNU",MID(Sheet1!A57,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A57&amp;",   """&amp;Sheet1!D57&amp;"\n""},","")</f>
+        <v>{0,MNU_IO,   "Input/Output\n"},</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="str">
-        <f>IF(MID(Sheet1!A58,1,3)="MNU","{0,"&amp;Sheet1!A58&amp;",   """&amp;Sheet1!E58&amp;"\n""},","")</f>
-        <v>{0,MNU_INFO,   "System information and some information about the value in the X-register\n"},</v>
+        <f>IF(AND(MID(Sheet1!A58,1,3)="MNU",MID(Sheet1!A58,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A58&amp;",   """&amp;Sheet1!D58&amp;"\n""},","")</f>
+        <v>{0,MNU_INFO,   "Information\n"},</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="str">
-        <f>IF(MID(Sheet1!A59,1,3)="MNU","{0,"&amp;Sheet1!A59&amp;",   """&amp;Sheet1!E59&amp;"\n""},","")</f>
-        <v>{0,MNU_INL_TST,   "Internal menu Inl. Tst ; part of test system\n"},</v>
+        <f>IF(AND(MID(Sheet1!A59,1,3)="MNU",MID(Sheet1!A59,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A59&amp;",   """&amp;Sheet1!D59&amp;"\n""},","")</f>
+        <v>{0,MNU_INL_TST,   "Inline test\n"},</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="str">
-        <f>IF(MID(Sheet1!A60,1,3)="MNU","{0,"&amp;Sheet1!A60&amp;",   """&amp;Sheet1!E60&amp;"\n""},","")</f>
-        <v>{0,MNU_INTS,   "Short integer functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A60,1,3)="MNU",MID(Sheet1!A60,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A60&amp;",   """&amp;Sheet1!D60&amp;"\n""},","")</f>
+        <v>{0,MNU_INTS,   "Integers\n"},</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="str">
-        <f>IF(MID(Sheet1!A61,1,3)="MNU","{0,"&amp;Sheet1!A61&amp;",   """&amp;Sheet1!E61&amp;"\n""},","")</f>
-        <v>{0,MNU_GAP_L,   "Select integer part separator\n"},</v>
+        <f>IF(AND(MID(Sheet1!A61,1,3)="MNU",MID(Sheet1!A61,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A61&amp;",   """&amp;Sheet1!D61&amp;"\n""},","")</f>
+        <v>{0,MNU_GAP_L,   "Select IP separator\n"},</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="str">
-        <f>IF(MID(Sheet1!A62,1,3)="MNU","{0,"&amp;Sheet1!A62&amp;",   """&amp;Sheet1!E62&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A62,1,3)="MNU",MID(Sheet1!A62,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A62&amp;",   """&amp;Sheet1!D62&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="str">
-        <f>IF(MID(Sheet1!A63,1,3)="MNU","{0,"&amp;Sheet1!A63&amp;",   """&amp;Sheet1!E63&amp;"\n""},","")</f>
-        <v>{0,MNU_ASN,   "Keyboard layouts\n"},</v>
+        <f>IF(AND(MID(Sheet1!A63,1,3)="MNU",MID(Sheet1!A63,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A63&amp;",   """&amp;Sheet1!D63&amp;"\n""},","")</f>
+        <v>{0,MNU_ASN,   "Keys\n"},</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="str">
-        <f>IF(MID(Sheet1!A64,1,3)="MNU","{0,"&amp;Sheet1!A64&amp;",   """&amp;Sheet1!E64&amp;"\n""},","")</f>
-        <v>{0,MNU_LINTS,   "Auto-generated catalog of variables of the specified type: long integer\n"},</v>
+        <f>IF(AND(MID(Sheet1!A64,1,3)="MNU",MID(Sheet1!A64,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A64&amp;",   """&amp;Sheet1!D64&amp;"\n""},","")</f>
+        <v>{0,MNU_LINTS,   "Longint variables\n"},</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="str">
-        <f>IF(MID(Sheet1!A65,1,3)="MNU","{0,"&amp;Sheet1!A65&amp;",   """&amp;Sheet1!E65&amp;"\n""},","")</f>
-        <v>{0,MNU_LGNRM,   "Log normal probability distribution\n"},</v>
+        <f>IF(AND(MID(Sheet1!A65,1,3)="MNU",MID(Sheet1!A65,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A65&amp;",   """&amp;Sheet1!D65&amp;"\n""},","")</f>
+        <v>{0,MNU_LGNRM,   "Log normal distribution\n"},</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="str">
-        <f>IF(MID(Sheet1!A66,1,3)="MNU","{0,"&amp;Sheet1!A66&amp;",   """&amp;Sheet1!E66&amp;"\n""},","")</f>
-        <v>{0,MNU_LOGIS,   "Logistic probability distribution\n"},</v>
+        <f>IF(AND(MID(Sheet1!A66,1,3)="MNU",MID(Sheet1!A66,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A66&amp;",   """&amp;Sheet1!D66&amp;"\n""},","")</f>
+        <v>{0,MNU_LOGIS,   "Logistic distribution\n"},</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="str">
-        <f>IF(MID(Sheet1!A67,1,3)="MNU","{0,"&amp;Sheet1!A67&amp;",   """&amp;Sheet1!E67&amp;"\n""},","")</f>
-        <v>{0,MNU_LOOP,   "Looping (programming) functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A67,1,3)="MNU",MID(Sheet1!A67,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A67&amp;",   """&amp;Sheet1!D67&amp;"\n""},","")</f>
+        <v>{0,MNU_LOOP,   "Looping\n"},</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="str">
-        <f>IF(MID(Sheet1!A68,1,3)="MNU","{0,"&amp;Sheet1!A68&amp;",   """&amp;Sheet1!E68&amp;"\n""},","")</f>
-        <v>{0,MNU_CONVM,   "Convert between units of mass\n"},</v>
+        <f>IF(AND(MID(Sheet1!A68,1,3)="MNU",MID(Sheet1!A68,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A68&amp;",   """&amp;Sheet1!D68&amp;"\n""},","")</f>
+        <v/>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="str">
-        <f>IF(MID(Sheet1!A69,1,3)="MNU","{0,"&amp;Sheet1!A69&amp;",   """&amp;Sheet1!E69&amp;"\n""},","")</f>
-        <v>{0,MNU_MATRS,   "Auto-generated catalog of variables of the specified type: matrix\n"},</v>
+        <f>IF(AND(MID(Sheet1!A69,1,3)="MNU",MID(Sheet1!A69,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A69&amp;",   """&amp;Sheet1!D69&amp;"\n""},","")</f>
+        <v>{0,MNU_MATRS,   "Matrix variables\n"},</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="str">
-        <f>IF(MID(Sheet1!A70,1,3)="MNU","{0,"&amp;Sheet1!A70&amp;",   """&amp;Sheet1!E70&amp;"\n""},","")</f>
-        <v>{0,MNU_MATX,   "Matrix functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A70,1,3)="MNU",MID(Sheet1!A70,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A70&amp;",   """&amp;Sheet1!D70&amp;"\n""},","")</f>
+        <v>{0,MNU_MATX,   "Matrix\n"},</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="str">
-        <f>IF(MID(Sheet1!A71,1,3)="MNU","{0,"&amp;Sheet1!A71&amp;",   """&amp;Sheet1!E71&amp;"\n""},","")</f>
-        <v>{0,MNU_MENUS,   "Catalog of all menus (including user defined menus)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A71,1,3)="MNU",MID(Sheet1!A71,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A71&amp;",   """&amp;Sheet1!D71&amp;"\n""},","")</f>
+        <v>{0,MNU_MENUS,   "MENUS\n"},</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="str">
-        <f>IF(MID(Sheet1!A72,1,3)="MNU","{0,"&amp;Sheet1!A72&amp;",   """&amp;Sheet1!E72&amp;"\n""},","")</f>
-        <v>{0,MNU_MISC,   "Time, temperature, torque, power and field ratio conversions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A72,1,3)="MNU",MID(Sheet1!A72,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A72&amp;",   """&amp;Sheet1!D72&amp;"\n""},","")</f>
+        <v>{0,MNU_MISC,   "Miscellaneous conversions\n"},</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="str">
-        <f>IF(MID(Sheet1!A73,1,3)="MNU","{0,"&amp;Sheet1!A73&amp;",   """&amp;Sheet1!E73&amp;"\n""},","")</f>
-        <v>{0,MNU_MODE,   "System (mode) settings with status indication and modification\n"},</v>
+        <f>IF(AND(MID(Sheet1!A73,1,3)="MNU",MID(Sheet1!A73,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A73&amp;",   """&amp;Sheet1!D73&amp;"\n""},","")</f>
+        <v>{0,MNU_MODE,   "Mode settings\n"},</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="str">
-        <f>IF(MID(Sheet1!A74,1,3)="MNU","{0,"&amp;Sheet1!A74&amp;",   """&amp;Sheet1!E74&amp;"\n""},","")</f>
-        <v>{0,MNU_MODEL,   "Model functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A74,1,3)="MNU",MID(Sheet1!A74,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A74&amp;",   """&amp;Sheet1!D74&amp;"\n""},","")</f>
+        <v>{0,MNU_MODEL,   "Model\n"},</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="str">
-        <f>IF(MID(Sheet1!A75,1,3)="MNU","{0,"&amp;Sheet1!A75&amp;",   """&amp;Sheet1!E75&amp;"\n""},","")</f>
-        <v>{0,MNU_MVAR,   "(Internal) menu MVAR for VarMNU\n"},</v>
+        <f>IF(AND(MID(Sheet1!A75,1,3)="MNU",MID(Sheet1!A75,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A75&amp;",   """&amp;Sheet1!D75&amp;"\n""},","")</f>
+        <v>{0,MNU_MVAR,   "MVAR\n"},</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="str">
-        <f>IF(MID(Sheet1!A76,1,3)="MNU","{0,"&amp;Sheet1!A76&amp;",   """&amp;Sheet1!E76&amp;"\n""},","")</f>
-        <v>{0,MNU_MyMenu,   "MyMenu is where to assign user selected functions or user selected or defined menus\n"},</v>
+        <f>IF(AND(MID(Sheet1!A76,1,3)="MNU",MID(Sheet1!A76,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A76&amp;",   """&amp;Sheet1!D76&amp;"\n""},","")</f>
+        <v>{0,MNU_MyMenu,   "MyMenu\n"},</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="str">
-        <f>IF(MID(Sheet1!A77,1,3)="MNU","{0,"&amp;Sheet1!A77&amp;",   """&amp;Sheet1!E77&amp;"\n""},","")</f>
-        <v>{0,MNU_MyAlpha,   "MyAlpha is where to assign special characters for easy entry\n"},</v>
+        <f>IF(AND(MID(Sheet1!A77,1,3)="MNU",MID(Sheet1!A77,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A77&amp;",   """&amp;Sheet1!D77&amp;"\n""},","")</f>
+        <v>{0,MNU_MyAlpha,   "MyAlpha\n"},</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="str">
-        <f>IF(MID(Sheet1!A78,1,3)="MNU","{0,"&amp;Sheet1!A78&amp;",   """&amp;Sheet1!E78&amp;"\n""},","")</f>
-        <v>{0,MNU_NBIN,   "Negative binomial probability distribution\n"},</v>
+        <f>IF(AND(MID(Sheet1!A78,1,3)="MNU",MID(Sheet1!A78,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A78&amp;",   """&amp;Sheet1!D78&amp;"\n""},","")</f>
+        <v>{0,MNU_NBIN,   "Negative binomial distribution\n"},</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="str">
-        <f>IF(MID(Sheet1!A79,1,3)="MNU","{0,"&amp;Sheet1!A79&amp;",   """&amp;Sheet1!E79&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A79,1,3)="MNU",MID(Sheet1!A79,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A79&amp;",   """&amp;Sheet1!D79&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="str">
-        <f>IF(MID(Sheet1!A80,1,3)="MNU","{0,"&amp;Sheet1!A80&amp;",   """&amp;Sheet1!E80&amp;"\n""},","")</f>
-        <v>{0,MNU_EQ_EDIT,   "Create new equation (previous equation pushed)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A80,1,3)="MNU",MID(Sheet1!A80,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A80&amp;",   """&amp;Sheet1!D80&amp;"\n""},","")</f>
+        <v>{0,MNU_EQ_EDIT,   "Equation editor\n"},</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="str">
-        <f>IF(MID(Sheet1!A81,1,3)="MNU","{0,"&amp;Sheet1!A81&amp;",   """&amp;Sheet1!E81&amp;"\n""},","")</f>
-        <v>{0,MNU_NORML,   "Normal probability distribution\n"},</v>
+        <f>IF(AND(MID(Sheet1!A81,1,3)="MNU",MID(Sheet1!A81,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A81&amp;",   """&amp;Sheet1!D81&amp;"\n""},","")</f>
+        <v>{0,MNU_NORML,   "Normal distribution\n"},</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="str">
-        <f>IF(MID(Sheet1!A82,1,3)="MNU","{0,"&amp;Sheet1!A82&amp;",   """&amp;Sheet1!E82&amp;"\n""},","")</f>
-        <v>{0,MNU_ORTHOG,   "Orthogonal polynomials\n"},</v>
+        <f>IF(AND(MID(Sheet1!A82,1,3)="MNU",MID(Sheet1!A82,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A82&amp;",   """&amp;Sheet1!D82&amp;"\n""},","")</f>
+        <v>{0,MNU_ORTHOG,   "Orthogonal\n"},</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="str">
-        <f>IF(MID(Sheet1!A83,1,3)="MNU","{0,"&amp;Sheet1!A83&amp;",   """&amp;Sheet1!E83&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A83,1,3)="MNU",MID(Sheet1!A83,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A83&amp;",   """&amp;Sheet1!D83&amp;"\n""},","")</f>
         <v>{0,MNU_PFN,   "Programming functions\n"},</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="str">
-        <f>IF(MID(Sheet1!A84,1,3)="MNU","{0,"&amp;Sheet1!A84&amp;",   """&amp;Sheet1!E84&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A84,1,3)="MNU",MID(Sheet1!A84,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A84&amp;",   """&amp;Sheet1!D84&amp;"\n""},","")</f>
         <v>{0,MNU_PFN_MORE,   "More programming functions\n"},</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="str">
-        <f>IF(MID(Sheet1!A85,1,3)="MNU","{0,"&amp;Sheet1!A85&amp;",   """&amp;Sheet1!E85&amp;"\n""},","")</f>
-        <v>{0,MNU_PARTS_C43,   "Functions on real and complex numbers\n"},</v>
+        <f>IF(AND(MID(Sheet1!A85,1,3)="MNU",MID(Sheet1!A85,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A85&amp;",   """&amp;Sheet1!D85&amp;"\n""},","")</f>
+        <v>{0,MNU_PARTS_C43,   "Part\n"},</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="str">
-        <f>IF(MID(Sheet1!A86,1,3)="MNU","{0,"&amp;Sheet1!A86&amp;",   """&amp;Sheet1!E86&amp;"\n""},","")</f>
-        <v>{0,MNU_PLOTTING,   "Plotting and summation functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A86,1,3)="MNU",MID(Sheet1!A86,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A86&amp;",   """&amp;Sheet1!D86&amp;"\n""},","")</f>
+        <v>{0,MNU_PLOTTING,   "Plotting\n"},</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="str">
-        <f>IF(MID(Sheet1!A87,1,3)="MNU","{0,"&amp;Sheet1!A87&amp;",   """&amp;Sheet1!E87&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A87,1,3)="MNU",MID(Sheet1!A87,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A87&amp;",   """&amp;Sheet1!D87&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="str">
-        <f>IF(MID(Sheet1!A88,1,3)="MNU","{0,"&amp;Sheet1!A88&amp;",   """&amp;Sheet1!E88&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A88,1,3)="MNU",MID(Sheet1!A88,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A88&amp;",   """&amp;Sheet1!D88&amp;"\n""},","")</f>
         <v>{0,MNU_PLOT_STAT,   "Plot statistics\n"},</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="str">
-        <f>IF(MID(Sheet1!A89,1,3)="MNU","{0,"&amp;Sheet1!A89&amp;",   """&amp;Sheet1!E89&amp;"\n""},","")</f>
-        <v>{0,MNU_POISS,   "Poisson probability distribution\n"},</v>
+        <f>IF(AND(MID(Sheet1!A89,1,3)="MNU",MID(Sheet1!A89,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A89&amp;",   """&amp;Sheet1!D89&amp;"\n""},","")</f>
+        <v>{0,MNU_POISS,   "Poisson distribution\n"},</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="str">
-        <f>IF(MID(Sheet1!A90,1,3)="MNU","{0,"&amp;Sheet1!A90&amp;",   """&amp;Sheet1!E90&amp;"\n""},","")</f>
-        <v>{0,MNU_CONVP,   "Convert between units of power\n"},</v>
+        <f>IF(AND(MID(Sheet1!A90,1,3)="MNU",MID(Sheet1!A90,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A90&amp;",   """&amp;Sheet1!D90&amp;"\n""},","")</f>
+        <v/>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="str">
-        <f>IF(MID(Sheet1!A91,1,3)="MNU","{0,"&amp;Sheet1!A91&amp;",   """&amp;Sheet1!E91&amp;"\n""},","")</f>
-        <v>{0,MNU_PRINT,   "Printing functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A91,1,3)="MNU",MID(Sheet1!A91,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A91&amp;",   """&amp;Sheet1!D91&amp;"\n""},","")</f>
+        <v>{0,MNU_PRINT,   "Printing\n"},</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="str">
-        <f>IF(MID(Sheet1!A92,1,3)="MNU","{0,"&amp;Sheet1!A92&amp;",   """&amp;Sheet1!E92&amp;"\n""},","")</f>
-        <v>{0,MNU_PROB,   "Probability functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A92,1,3)="MNU",MID(Sheet1!A92,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A92&amp;",   """&amp;Sheet1!D92&amp;"\n""},","")</f>
+        <v>{0,MNU_PROB,   "Probability\n"},</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="str">
-        <f>IF(MID(Sheet1!A93,1,3)="MNU","{0,"&amp;Sheet1!A93&amp;",   """&amp;Sheet1!E93&amp;"\n""},","")</f>
-        <v>{0,MNU_PROG,   "Presented in TAM menus for commands accessing labels\n"},</v>
+        <f>IF(AND(MID(Sheet1!A93,1,3)="MNU",MID(Sheet1!A93,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A93&amp;",   """&amp;Sheet1!D93&amp;"\n""},","")</f>
+        <v>{0,MNU_PROG,   "PROG\n"},</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="str">
-        <f>IF(MID(Sheet1!A94,1,3)="MNU","{0,"&amp;Sheet1!A94&amp;",   """&amp;Sheet1!E94&amp;"\n""},","")</f>
-        <v>{0,MNU_PROGS,   "Auto-generated catalog of programs\n"},</v>
+        <f>IF(AND(MID(Sheet1!A94,1,3)="MNU",MID(Sheet1!A94,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A94&amp;",   """&amp;Sheet1!D94&amp;"\n""},","")</f>
+        <v>{0,MNU_PROGS,   "Programs\n"},</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="str">
-        <f>IF(MID(Sheet1!A95,1,3)="MNU","{0,"&amp;Sheet1!A95&amp;",   """&amp;Sheet1!E95&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A95,1,3)="MNU",MID(Sheet1!A95,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A95&amp;",   """&amp;Sheet1!D95&amp;"\n""},","")</f>
         <v>{0,MNU_RADIX,   "Select radix\n"},</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="str">
-        <f>IF(MID(Sheet1!A96,1,3)="MNU","{0,"&amp;Sheet1!A96&amp;",   """&amp;Sheet1!E96&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A96,1,3)="MNU",MID(Sheet1!A96,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A96&amp;",   """&amp;Sheet1!D96&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="str">
-        <f>IF(MID(Sheet1!A97,1,3)="MNU","{0,"&amp;Sheet1!A97&amp;",   """&amp;Sheet1!E97&amp;"\n""},","")</f>
-        <v>{0,MNU_RAM,   "Auto-generated catalog of programs in RAM (main) memory\n"},</v>
+        <f>IF(AND(MID(Sheet1!A97,1,3)="MNU",MID(Sheet1!A97,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A97&amp;",   """&amp;Sheet1!D97&amp;"\n""},","")</f>
+        <v>{0,MNU_RAM,   "RAM programs\n"},</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="str">
-        <f>IF(MID(Sheet1!A98,1,3)="MNU","{0,"&amp;Sheet1!A98&amp;",   """&amp;Sheet1!E98&amp;"\n""},","")</f>
-        <v>{0,MNU_PARTS,   "Functions on real and complex numbers\n"},</v>
+        <f>IF(AND(MID(Sheet1!A98,1,3)="MNU",MID(Sheet1!A98,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A98&amp;",   """&amp;Sheet1!D98&amp;"\n""},","")</f>
+        <v>{0,MNU_PARTS,   "Real\n"},</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="str">
-        <f>IF(MID(Sheet1!A99,1,3)="MNU","{0,"&amp;Sheet1!A99&amp;",   """&amp;Sheet1!E99&amp;"\n""},","")</f>
-        <v>{0,MNU_REALS,   "Auto-generated catalog of variables of the specified type: real\n"},</v>
+        <f>IF(AND(MID(Sheet1!A99,1,3)="MNU",MID(Sheet1!A99,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A99&amp;",   """&amp;Sheet1!D99&amp;"\n""},","")</f>
+        <v>{0,MNU_REALS,   "Real variables\n"},</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="str">
-        <f>IF(MID(Sheet1!A100,1,3)="MNU","{0,"&amp;Sheet1!A100&amp;",   """&amp;Sheet1!E100&amp;"\n""},","")</f>
-        <v>{0,MNU_REGR,   "Regression functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A100,1,3)="MNU",MID(Sheet1!A100,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A100&amp;",   """&amp;Sheet1!D100&amp;"\n""},","")</f>
+        <v>{0,MNU_REGR,   "Regression\n"},</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="str">
-        <f>IF(MID(Sheet1!A101,1,3)="MNU","{0,"&amp;Sheet1!A101&amp;",   """&amp;Sheet1!E101&amp;"\n""},","")</f>
-        <v>{0,MNU_SINTS,   "Auto-generated catalog of variables of the specified type: short integer\n"},</v>
+        <f>IF(AND(MID(Sheet1!A101,1,3)="MNU",MID(Sheet1!A101,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A101&amp;",   """&amp;Sheet1!D101&amp;"\n""},","")</f>
+        <v>{0,MNU_SINTS,   "Shortint variables\n"},</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="str">
-        <f>IF(MID(Sheet1!A102,1,3)="MNU","{0,"&amp;Sheet1!A102&amp;",   """&amp;Sheet1!E102&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A102,1,3)="MNU",MID(Sheet1!A102,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A102&amp;",   """&amp;Sheet1!D102&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="str">
-        <f>IF(MID(Sheet1!A103,1,3)="MNU","{0,"&amp;Sheet1!A103&amp;",   """&amp;Sheet1!E103&amp;"\n""},","")</f>
-        <v>{0,MNU_PLOT,   "Scatter plot of measurments\n"},</v>
+        <f>IF(AND(MID(Sheet1!A103,1,3)="MNU",MID(Sheet1!A103,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A103&amp;",   """&amp;Sheet1!D103&amp;"\n""},","")</f>
+        <v>{0,MNU_PLOT,   "Scatter plot\n"},</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="str">
-        <f>IF(MID(Sheet1!A104,1,3)="MNU","{0,"&amp;Sheet1!A104&amp;",   """&amp;Sheet1!E104&amp;"\n""},","")</f>
-        <v>{0,MNU_SETUP,   "System (mode) settings with status indication and modification\n"},</v>
+        <f>IF(AND(MID(Sheet1!A104,1,3)="MNU",MID(Sheet1!A104,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A104&amp;",   """&amp;Sheet1!D104&amp;"\n""},","")</f>
+        <v>{0,MNU_SETUP,   "Setup\n"},</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="str">
-        <f>IF(MID(Sheet1!A105,1,3)="MNU","{0,"&amp;Sheet1!A105&amp;",   """&amp;Sheet1!E105&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A105,1,3)="MNU",MID(Sheet1!A105,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A105&amp;",   """&amp;Sheet1!D105&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="str">
-        <f>IF(MID(Sheet1!A106,1,3)="MNU","{0,"&amp;Sheet1!A106&amp;",   """&amp;Sheet1!E106&amp;"\n""},","")</f>
-        <v>{0,MNU_SIMQ,   "Matrix simultaneous equations functions (Mat A • Mat X = Mat B)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A106,1,3)="MNU",MID(Sheet1!A106,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A106&amp;",   """&amp;Sheet1!D106&amp;"\n""},","")</f>
+        <v>{0,MNU_SIMQ,   "Matrix simultaneous equations\n"},</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="str">
-        <f>IF(MID(Sheet1!A107,1,3)="MNU","{0,"&amp;Sheet1!A107&amp;",   """&amp;Sheet1!E107&amp;"\n""},","")</f>
-        <v>{0,MNU_Solver,   "Solver, with iteration counter, interrupt by keypress ; tolerance set by SDIGS\n"},</v>
+        <f>IF(AND(MID(Sheet1!A107,1,3)="MNU",MID(Sheet1!A107,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A107&amp;",   """&amp;Sheet1!D107&amp;"\n""},","")</f>
+        <v>{0,MNU_Solver,   "Solver\n"},</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="str">
-        <f>IF(MID(Sheet1!A108,1,3)="MNU","{0,"&amp;Sheet1!A108&amp;",   """&amp;Sheet1!E108&amp;"\n""},","")</f>
-        <v>{0,MNU_CONVS,   "Convert between units of speed\n"},</v>
+        <f>IF(AND(MID(Sheet1!A108,1,3)="MNU",MID(Sheet1!A108,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A108&amp;",   """&amp;Sheet1!D108&amp;"\n""},","")</f>
+        <v/>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="str">
-        <f>IF(MID(Sheet1!A109,1,3)="MNU","{0,"&amp;Sheet1!A109&amp;",   """&amp;Sheet1!E109&amp;"\n""},","")</f>
-        <v>{0,MNU_STAT,   "Statistics functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A109,1,3)="MNU",MID(Sheet1!A109,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A109&amp;",   """&amp;Sheet1!D109&amp;"\n""},","")</f>
+        <v>{0,MNU_STAT,   "Statistics\n"},</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="str">
-        <f>IF(MID(Sheet1!A110,1,3)="MNU","{0,"&amp;Sheet1!A110&amp;",   """&amp;Sheet1!E110&amp;"\n""},","")</f>
-        <v>{0,MNU_STK,   "Stack functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A110,1,3)="MNU",MID(Sheet1!A110,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A110&amp;",   """&amp;Sheet1!D110&amp;"\n""},","")</f>
+        <v>{0,MNU_STK,   "Stack\n"},</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="str">
-        <f>IF(MID(Sheet1!A111,1,3)="MNU","{0,"&amp;Sheet1!A111&amp;",   """&amp;Sheet1!E111&amp;"\n""},","")</f>
-        <v>{0,MNU_STRINGS,   "Auto-generated catalog of variables of the specified type: string\n"},</v>
+        <f>IF(AND(MID(Sheet1!A111,1,3)="MNU",MID(Sheet1!A111,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A111&amp;",   """&amp;Sheet1!D111&amp;"\n""},","")</f>
+        <v>{0,MNU_STRINGS,   "String variables\n"},</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="str">
-        <f>IF(MID(Sheet1!A112,1,3)="MNU","{0,"&amp;Sheet1!A112&amp;",   """&amp;Sheet1!E112&amp;"\n""},","")</f>
-        <v>{0,MNU_SUMS_C43,   "Summation and plotting functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A112,1,3)="MNU",MID(Sheet1!A112,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A112&amp;",   """&amp;Sheet1!D112&amp;"\n""},","")</f>
+        <v>{0,MNU_SUMS_C43,   "Sum(s)\n"},</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="str">
-        <f>IF(MID(Sheet1!A113,1,3)="MNU","{0,"&amp;Sheet1!A113&amp;",   """&amp;Sheet1!E113&amp;"\n""},","")</f>
-        <v>{0,MNU_SYSFL,   "Presented in TAM menus for commands accessing system flags\n"},</v>
+        <f>IF(AND(MID(Sheet1!A113,1,3)="MNU",MID(Sheet1!A113,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A113&amp;",   """&amp;Sheet1!D113&amp;"\n""},","")</f>
+        <v>{0,MNU_SYSFL,   "System flags\n"},</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="str">
-        <f>IF(MID(Sheet1!A114,1,3)="MNU","{0,"&amp;Sheet1!A114&amp;",   """&amp;Sheet1!E114&amp;"\n""},","")</f>
-        <v>{0,MNU_T,   "Student's t probability distribution\n"},</v>
+        <f>IF(AND(MID(Sheet1!A114,1,3)="MNU",MID(Sheet1!A114,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A114&amp;",   """&amp;Sheet1!D114&amp;"\n""},","")</f>
+        <v>{0,MNU_T,   "Student's t distribution\n"},</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="str">
-        <f>IF(MID(Sheet1!A115,1,3)="MNU","{0,"&amp;Sheet1!A115&amp;",   """&amp;Sheet1!E115&amp;"\n""},","")</f>
-        <v>{0,MNU_TAM,   "Transient alpha mode is activated for trailing input (general)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A115,1,3)="MNU",MID(Sheet1!A115,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A115&amp;",   """&amp;Sheet1!D115&amp;"\n""},","")</f>
+        <v>{0,MNU_TAM,   "TAM mode\n"},</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="str">
-        <f>IF(MID(Sheet1!A116,1,3)="MNU","{0,"&amp;Sheet1!A116&amp;",   """&amp;Sheet1!E116&amp;"\n""},","")</f>
-        <v>{0,MNU_TAMCMP,   "Transient alpha mode is activated for trailing input (compare)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A116,1,3)="MNU",MID(Sheet1!A116,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A116&amp;",   """&amp;Sheet1!D116&amp;"\n""},","")</f>
+        <v>{0,MNU_TAMCMP,   "TAM mode CMP\n"},</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="str">
-        <f>IF(MID(Sheet1!A117,1,3)="MNU","{0,"&amp;Sheet1!A117&amp;",   """&amp;Sheet1!E117&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A117,1,3)="MNU",MID(Sheet1!A117,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A117&amp;",   """&amp;Sheet1!D117&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="str">
-        <f>IF(MID(Sheet1!A118,1,3)="MNU","{0,"&amp;Sheet1!A118&amp;",   """&amp;Sheet1!E118&amp;"\n""},","")</f>
-        <v>{0,MNU_TAMFLAG,   "Transient alpha mode is activated for trailing input (flag)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A118,1,3)="MNU",MID(Sheet1!A118,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A118&amp;",   """&amp;Sheet1!D118&amp;"\n""},","")</f>
+        <v>{0,MNU_TAMFLAG,   "TAM mode FLAG\n"},</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="str">
-        <f>IF(MID(Sheet1!A119,1,3)="MNU","{0,"&amp;Sheet1!A119&amp;",   """&amp;Sheet1!E119&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A119,1,3)="MNU",MID(Sheet1!A119,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A119&amp;",   """&amp;Sheet1!D119&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="str">
-        <f>IF(MID(Sheet1!A120,1,3)="MNU","{0,"&amp;Sheet1!A120&amp;",   """&amp;Sheet1!E120&amp;"\n""},","")</f>
-        <v>{0,MNU_TAMLABEL,   "Transient alpha mode is activated for trailing input (LBL/GTO/XEQ)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A120,1,3)="MNU",MID(Sheet1!A120,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A120&amp;",   """&amp;Sheet1!D120&amp;"\n""},","")</f>
+        <v>{0,MNU_TAMLABEL,   "TAM mode LABEL\n"},</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="str">
-        <f>IF(MID(Sheet1!A121,1,3)="MNU","{0,"&amp;Sheet1!A121&amp;",   """&amp;Sheet1!E121&amp;"\n""},","")</f>
-        <v>{0,MNU_TAMLBLALPHA,   "Transient alpha mode is activated for trailing input (LBL/GTO/XEQ + alpha)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A121,1,3)="MNU",MID(Sheet1!A121,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A121&amp;",   """&amp;Sheet1!D121&amp;"\n""},","")</f>
+        <v>{0,MNU_TAMLBLALPHA,   "TAM mode LABEL/alpha\n"},</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="str">
-        <f>IF(MID(Sheet1!A122,1,3)="MNU","{0,"&amp;Sheet1!A122&amp;",   """&amp;Sheet1!E122&amp;"\n""},","")</f>
-        <v>{0,MNU_TAMNONREG,   "Transient alpha mode is activated for trailing input (value)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A122,1,3)="MNU",MID(Sheet1!A122,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A122&amp;",   """&amp;Sheet1!D122&amp;"\n""},","")</f>
+        <v>{0,MNU_TAMNONREG,   "TAM mode VALUE\n"},</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="str">
-        <f>IF(MID(Sheet1!A123,1,3)="MNU","{0,"&amp;Sheet1!A123&amp;",   """&amp;Sheet1!E123&amp;"\n""},","")</f>
-        <v>{0,MNU_TAMNONREGIND,   "Transient alpha mode is activated for trailing input (indirect)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A123,1,3)="MNU",MID(Sheet1!A123,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A123&amp;",   """&amp;Sheet1!D123&amp;"\n""},","")</f>
+        <v>{0,MNU_TAMNONREGIND,   "TAM mode INDIRECT\n"},</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="str">
-        <f>IF(MID(Sheet1!A124,1,3)="MNU","{0,"&amp;Sheet1!A124&amp;",   """&amp;Sheet1!E124&amp;"\n""},","")</f>
-        <v>{0,MNU_TAMSHUFFLE,   "Transient alpha mode is activated for trailing input (shuffle)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A124,1,3)="MNU",MID(Sheet1!A124,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A124&amp;",   """&amp;Sheet1!D124&amp;"\n""},","")</f>
+        <v>{0,MNU_TAMSHUFFLE,   "TAM mode SHUFFLE\n"},</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="str">
-        <f>IF(MID(Sheet1!A125,1,3)="MNU","{0,"&amp;Sheet1!A125&amp;",   """&amp;Sheet1!E125&amp;"\n""},","")</f>
-        <v>{0,MNU_TAMSTORCL,   "Transient alpha mode is activated for trailing input (STO, RCL)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A125,1,3)="MNU",MID(Sheet1!A125,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A125&amp;",   """&amp;Sheet1!D125&amp;"\n""},","")</f>
+        <v>{0,MNU_TAMSTORCL,   "TAM mode STORCL\n"},</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="str">
-        <f>IF(MID(Sheet1!A126,1,3)="MNU","{0,"&amp;Sheet1!A126&amp;",   """&amp;Sheet1!E126&amp;"\n""},","")</f>
-        <v>{0,MNU_TAMSRALPHA,   "Transient alpha mode is activated for trailing input (STO, RCL + alpha)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A126,1,3)="MNU",MID(Sheet1!A126,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A126&amp;",   """&amp;Sheet1!D126&amp;"\n""},","")</f>
+        <v>{0,MNU_TAMSRALPHA,   "TAM mode STORCL/alpha\n"},</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="str">
-        <f>IF(MID(Sheet1!A127,1,3)="MNU","{0,"&amp;Sheet1!A127&amp;",   """&amp;Sheet1!E127&amp;"\n""},","")</f>
-        <v>{0,MNU_TEST,   "Testing functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A127,1,3)="MNU",MID(Sheet1!A127,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A127&amp;",   """&amp;Sheet1!D127&amp;"\n""},","")</f>
+        <v>{0,MNU_TEST,   "Testing\n"},</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="str">
-        <f>IF(MID(Sheet1!A128,1,3)="MNU","{0,"&amp;Sheet1!A128&amp;",   """&amp;Sheet1!E128&amp;"\n""},","")</f>
-        <v>{0,MNU_TIMES,   "Auto-generated catalog of variables of the specified type: time\n"},</v>
+        <f>IF(AND(MID(Sheet1!A128,1,3)="MNU",MID(Sheet1!A128,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A128&amp;",   """&amp;Sheet1!D128&amp;"\n""},","")</f>
+        <v>{0,MNU_TIMES,   "Time variables\n"},</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="str">
-        <f>IF(MID(Sheet1!A129,1,3)="MNU","{0,"&amp;Sheet1!A129&amp;",   """&amp;Sheet1!E129&amp;"\n""},","")</f>
-        <v>{0,MNU_TRG_C47,   "Trigonometry and hyperbolic functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A129,1,3)="MNU",MID(Sheet1!A129,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A129&amp;",   """&amp;Sheet1!D129&amp;"\n""},","")</f>
+        <v>{0,MNU_TRG_C47,   "Trigonometry\n"},</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="str">
-        <f>IF(MID(Sheet1!A130,1,3)="MNU","{0,"&amp;Sheet1!A130&amp;",   """&amp;Sheet1!E130&amp;"\n""},","")</f>
-        <v>{0,MNU_TRG_C47_MORE,   "Extended trigonometry (and access to hyperbolic) functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A130,1,3)="MNU",MID(Sheet1!A130,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A130&amp;",   """&amp;Sheet1!D130&amp;"\n""},","")</f>
+        <v>{0,MNU_TRG_C47_MORE,   "More trig/hyperbolics\n"},</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="str">
-        <f>IF(MID(Sheet1!A131,1,3)="MNU","{0,"&amp;Sheet1!A131&amp;",   """&amp;Sheet1!E131&amp;"\n""},","")</f>
-        <v>{0,MNU_TRG,   "Trigonometry functions (other layouts)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A131,1,3)="MNU",MID(Sheet1!A131,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A131&amp;",   """&amp;Sheet1!D131&amp;"\n""},","")</f>
+        <v>{0,MNU_TRG,   "Trigonometry\n"},</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="str">
-        <f>IF(MID(Sheet1!A132,1,3)="MNU","{0,"&amp;Sheet1!A132&amp;",   """&amp;Sheet1!E132&amp;"\n""},","")</f>
-        <v>{0,MNU_TRI,   "Trigonometry and hyperbolic functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A132,1,3)="MNU",MID(Sheet1!A132,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A132&amp;",   """&amp;Sheet1!D132&amp;"\n""},","")</f>
+        <v>{0,MNU_TRI,   "Trigonometry\n"},</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="str">
-        <f>IF(MID(Sheet1!A133,1,3)="MNU","{0,"&amp;Sheet1!A133&amp;",   """&amp;Sheet1!E133&amp;"\n""},","")</f>
-        <v>{0,MNU_TVM,   "Time value of money functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A133,1,3)="MNU",MID(Sheet1!A133,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A133&amp;",   """&amp;Sheet1!D133&amp;"\n""},","")</f>
+        <v>{0,MNU_TVM,   "Time value of money\n"},</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="str">
-        <f>IF(MID(Sheet1!A134,1,3)="MNU","{0,"&amp;Sheet1!A134&amp;",   """&amp;Sheet1!E134&amp;"\n""},","")</f>
-        <v>{0,MNU_UNITCONV_C43,   "Unit conversions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A134,1,3)="MNU",MID(Sheet1!A134,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A134&amp;",   """&amp;Sheet1!D134&amp;"\n""},","")</f>
+        <v>{0,MNU_UNITCONV_C43,   "Unit\n"},</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="str">
-        <f>IF(MID(Sheet1!A135,1,3)="MNU","{0,"&amp;Sheet1!A135&amp;",   """&amp;Sheet1!E135&amp;"\n""},","")</f>
-        <v>{0,MNU_VAR,   "Presented in TAM menus for commands accessing variables\n"},</v>
+        <f>IF(AND(MID(Sheet1!A135,1,3)="MNU",MID(Sheet1!A135,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A135&amp;",   """&amp;Sheet1!D135&amp;"\n""},","")</f>
+        <v>{0,MNU_VAR,   "VAR\n"},</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="str">
-        <f>IF(MID(Sheet1!A136,1,3)="MNU","{0,"&amp;Sheet1!A136&amp;",   """&amp;Sheet1!E136&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A136,1,3)="MNU",MID(Sheet1!A136,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A136&amp;",   """&amp;Sheet1!D136&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="str">
-        <f>IF(MID(Sheet1!A137,1,3)="MNU","{0,"&amp;Sheet1!A137&amp;",   """&amp;Sheet1!E137&amp;"\n""},","")</f>
-        <v>{0,MNU_VARS,   "Auto-generated catalog of variables\n"},</v>
+        <f>IF(AND(MID(Sheet1!A137,1,3)="MNU",MID(Sheet1!A137,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A137&amp;",   """&amp;Sheet1!D137&amp;"\n""},","")</f>
+        <v>{0,MNU_VARS,   "Variables\n"},</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="str">
-        <f>IF(MID(Sheet1!A138,1,3)="MNU","{0,"&amp;Sheet1!A138&amp;",   """&amp;Sheet1!E138&amp;"\n""},","")</f>
-        <v>{0,MNU_CONVV,   "Convert between units of volume\n"},</v>
+        <f>IF(AND(MID(Sheet1!A138,1,3)="MNU",MID(Sheet1!A138,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A138&amp;",   """&amp;Sheet1!D138&amp;"\n""},","")</f>
+        <v/>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="str">
-        <f>IF(MID(Sheet1!A139,1,3)="MNU","{0,"&amp;Sheet1!A139&amp;",   """&amp;Sheet1!E139&amp;"\n""},","")</f>
-        <v>{0,MNU_WEIBL,   "Weibull probability distribution\n"},</v>
+        <f>IF(AND(MID(Sheet1!A139,1,3)="MNU",MID(Sheet1!A139,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A139&amp;",   """&amp;Sheet1!D139&amp;"\n""},","")</f>
+        <v>{0,MNU_WEIBL,   "Weibull distribution\n"},</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="str">
-        <f>IF(MID(Sheet1!A140,1,3)="MNU","{0,"&amp;Sheet1!A140&amp;",   """&amp;Sheet1!E140&amp;"\n""},","")</f>
-        <v>{0,MNU_XFN,   "Extended functions (Bessel, Bernouilli, Gamma, Elliptical, Orthogonal, etc.)\n"},</v>
+        <f>IF(AND(MID(Sheet1!A140,1,3)="MNU",MID(Sheet1!A140,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A140&amp;",   """&amp;Sheet1!D140&amp;"\n""},","")</f>
+        <v>{0,MNU_XFN,   "Extended functions\n"},</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="str">
-        <f>IF(MID(Sheet1!A141,1,3)="MNU","{0,"&amp;Sheet1!A141&amp;",   """&amp;Sheet1!E141&amp;"\n""},","")</f>
-        <v>{0,MNU_XEQ,   "Menu of predefined functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A141,1,3)="MNU",MID(Sheet1!A141,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A141&amp;",   """&amp;Sheet1!D141&amp;"\n""},","")</f>
+        <v>{0,MNU_XEQ,   "XEQM\n"},</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="str">
-        <f>IF(MID(Sheet1!A142,1,3)="MNU","{0,"&amp;Sheet1!A142&amp;",   """&amp;Sheet1!E142&amp;"\n""},","")</f>
-        <v>{0,MNU_XXEQ,   "XXEQ menu\n"},</v>
+        <f>IF(AND(MID(Sheet1!A142,1,3)="MNU",MID(Sheet1!A142,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A142&amp;",   """&amp;Sheet1!D142&amp;"\n""},","")</f>
+        <v>{0,MNU_XXEQ,   "XXEQ\n"},</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="str">
-        <f>IF(MID(Sheet1!A143,1,3)="MNU","{0,"&amp;Sheet1!A143&amp;",   """&amp;Sheet1!E143&amp;"\n""},","")</f>
-        <v>{0,MNU_ALPHA,   "Alpha menu is used to enter, edit and clear alpha input\n"},</v>
+        <f>IF(AND(MID(Sheet1!A143,1,3)="MNU",MID(Sheet1!A143,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A143&amp;",   """&amp;Sheet1!D143&amp;"\n""},","")</f>
+        <v>{0,MNU_ALPHA,   "Alpha input\n"},</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="str">
-        <f>IF(MID(Sheet1!A144,1,3)="MNU","{0,"&amp;Sheet1!A144&amp;",   """&amp;Sheet1!E144&amp;"\n""},","")</f>
-        <v>{0,MNU_ALPHA_OMEGA,   "Uppercase Greek characters\n"},</v>
+        <f>IF(AND(MID(Sheet1!A144,1,3)="MNU",MID(Sheet1!A144,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A144&amp;",   """&amp;Sheet1!D144&amp;"\n""},","")</f>
+        <v>{0,MNU_ALPHA_OMEGA,   "ALPHA..OMEGA\n"},</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="str">
-        <f>IF(MID(Sheet1!A145,1,3)="MNU","{0,"&amp;Sheet1!A145&amp;",   """&amp;Sheet1!E145&amp;"\n""},","")</f>
-        <v>{0,MNU_alpha_omega.lo,   "Lowercase Greek characters\n"},</v>
+        <f>IF(AND(MID(Sheet1!A145,1,3)="MNU",MID(Sheet1!A145,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A145&amp;",   """&amp;Sheet1!D145&amp;"\n""},","")</f>
+        <v>{0,MNU_alpha_omega.lo,   "alpha..omega\n"},</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="str">
-        <f>IF(MID(Sheet1!A146,1,3)="MNU","{0,"&amp;Sheet1!A146&amp;",   """&amp;Sheet1!E146&amp;"\n""},","")</f>
-        <v>{0,MNU_ALPHAFN,   "Alpha (string) functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A146,1,3)="MNU",MID(Sheet1!A146,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A146&amp;",   """&amp;Sheet1!D146&amp;"\n""},","")</f>
+        <v>{0,MNU_ALPHAFN,   "Alpha string\n"},</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="str">
-        <f>IF(MID(Sheet1!A147,1,3)="MNU","{0,"&amp;Sheet1!A147&amp;",   """&amp;Sheet1!E147&amp;"\n""},","")</f>
-        <v>{0,MNU_ALPHADOT,   "Special characters\n"},</v>
+        <f>IF(AND(MID(Sheet1!A147,1,3)="MNU",MID(Sheet1!A147,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A147&amp;",   """&amp;Sheet1!D147&amp;"\n""},","")</f>
+        <v>{0,MNU_ALPHADOT,   "Alpha dot\n"},</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="str">
-        <f>IF(MID(Sheet1!A148,1,3)="MNU","{0,"&amp;Sheet1!A148&amp;",   """&amp;Sheet1!E148&amp;"\n""},","")</f>
-        <v>{0,MNU_ALPHAINTL,   "International characters\n"},</v>
+        <f>IF(AND(MID(Sheet1!A148,1,3)="MNU",MID(Sheet1!A148,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A148&amp;",   """&amp;Sheet1!D148&amp;"\n""},","")</f>
+        <v>{0,MNU_ALPHAINTL,   "Alpha international\n"},</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="str">
-        <f>IF(MID(Sheet1!A149,1,3)="MNU","{0,"&amp;Sheet1!A149&amp;",   """&amp;Sheet1!E149&amp;"\n""},","")</f>
-        <v>{0,MNU_ALPHAINTL.lo,   "Lowercase international characters\n"},</v>
+        <f>IF(AND(MID(Sheet1!A149,1,3)="MNU",MID(Sheet1!A149,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A149&amp;",   """&amp;Sheet1!D149&amp;"\n""},","")</f>
+        <v>{0,MNU_ALPHAINTL.lo,   "alpha international\n"},</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="str">
-        <f>IF(MID(Sheet1!A150,1,3)="MNU","{0,"&amp;Sheet1!A150&amp;",   """&amp;Sheet1!E150&amp;"\n""},","")</f>
-        <v>{0,MNU_ALPHAMATH,   "Mathematical symbols\n"},</v>
+        <f>IF(AND(MID(Sheet1!A150,1,3)="MNU",MID(Sheet1!A150,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A150&amp;",   """&amp;Sheet1!D150&amp;"\n""},","")</f>
+        <v>{0,MNU_ALPHAMATH,   "Alpha Math\n"},</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="str">
-        <f>IF(MID(Sheet1!A151,1,3)="MNU","{0,"&amp;Sheet1!A151&amp;",   """&amp;Sheet1!E151&amp;"\n""},","")</f>
-        <v>{0,MNU_ALPHAFN_C43,   "Alpha (string) functions\n"},</v>
+        <f>IF(AND(MID(Sheet1!A151,1,3)="MNU",MID(Sheet1!A151,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A151&amp;",   """&amp;Sheet1!D151&amp;"\n""},","")</f>
+        <v>{0,MNU_ALPHAFN_C43,   "Alpha string\n"},</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="str">
-        <f>IF(MID(Sheet1!A152,1,3)="MNU","{0,"&amp;Sheet1!A152&amp;",   """&amp;Sheet1!E152&amp;"\n""},","")</f>
-        <v>{0,MNU_ASN_N,   "Submenu for special key assignments to Sigma+ key in normal mode\n"},</v>
+        <f>IF(AND(MID(Sheet1!A152,1,3)="MNU",MID(Sheet1!A152,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A152&amp;",   """&amp;Sheet1!D152&amp;"\n""},","")</f>
+        <v>{0,MNU_ASN_N,   "Special key assignments\n"},</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="str">
-        <f>IF(MID(Sheet1!A153,1,3)="MNU","{0,"&amp;Sheet1!A153&amp;",   """&amp;Sheet1!E153&amp;"\n""},","")</f>
-        <v>{0,MNU_STDNORML,   "Standard normal probability distribution\n"},</v>
+        <f>IF(AND(MID(Sheet1!A153,1,3)="MNU",MID(Sheet1!A153,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A153&amp;",   """&amp;Sheet1!D153&amp;"\n""},","")</f>
+        <v>{0,MNU_STDNORML,   "Standard normal (probability)\n"},</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="str">
-        <f>IF(MID(Sheet1!A154,1,3)="MNU","{0,"&amp;Sheet1!A154&amp;",   """&amp;Sheet1!E154&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A154,1,3)="MNU",MID(Sheet1!A154,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A154&amp;",   """&amp;Sheet1!D154&amp;"\n""},","")</f>
         <v>{0,MNU_CHI2,   "χⅢ distribution\n"},</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="str">
-        <f>IF(MID(Sheet1!A155,1,3)="MNU","{0,"&amp;Sheet1!A155&amp;",   """&amp;Sheet1!E155&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A155,1,3)="MNU",MID(Sheet1!A155,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A155&amp;",   """&amp;Sheet1!D155&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="str">
-        <f>IF(MID(Sheet1!A156,1,3)="MNU","{0,"&amp;Sheet1!A156&amp;",   """&amp;Sheet1!E156&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A156,1,3)="MNU",MID(Sheet1!A156,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A156&amp;",   """&amp;Sheet1!D156&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="str">
-        <f>IF(MID(Sheet1!A157,1,3)="MNU","{0,"&amp;Sheet1!A157&amp;",   """&amp;Sheet1!E157&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A157,1,3)="MNU",MID(Sheet1!A157,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A157&amp;",   """&amp;Sheet1!D157&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="str">
-        <f>IF(MID(Sheet1!A158,1,3)="MNU","{0,"&amp;Sheet1!A158&amp;",   """&amp;Sheet1!E158&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A158,1,3)="MNU",MID(Sheet1!A158,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A158&amp;",   """&amp;Sheet1!D158&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="str">
-        <f>IF(MID(Sheet1!A159,1,3)="MNU","{0,"&amp;Sheet1!A159&amp;",   """&amp;Sheet1!E159&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A159,1,3)="MNU",MID(Sheet1!A159,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A159&amp;",   """&amp;Sheet1!D159&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="str">
-        <f>IF(MID(Sheet1!A160,1,3)="MNU","{0,"&amp;Sheet1!A160&amp;",   """&amp;Sheet1!E160&amp;"\n""},","")</f>
+        <f>IF(AND(MID(Sheet1!A160,1,3)="MNU",MID(Sheet1!A160,1,8)&lt;&gt;"MNU_CONV"),"{0,"&amp;Sheet1!A160&amp;",   """&amp;Sheet1!D160&amp;"\n""},","")</f>
         <v/>
       </c>
     </row>

</xml_diff>